<commit_message>
added code for browserstack
</commit_message>
<xml_diff>
--- a/artifact/data/MyFirstProject.data.xlsx
+++ b/artifact/data/MyFirstProject.data.xlsx
@@ -51,7 +51,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="66">
   <si>
     <t>true</t>
   </si>
@@ -198,6 +198,57 @@
   </si>
   <si>
     <t>HR Management System | HR Management Software | OrangeHRM</t>
+  </si>
+  <si>
+    <t>2</t>
+  </si>
+  <si>
+    <t>nexial.browser</t>
+  </si>
+  <si>
+    <t>chrome</t>
+  </si>
+  <si>
+    <t>nexial.browserstack.username</t>
+  </si>
+  <si>
+    <t>krishnas5</t>
+  </si>
+  <si>
+    <t>nexial.browserstack.automatekey</t>
+  </si>
+  <si>
+    <t>GqsYLXXeCWk5pYLDGzeQ</t>
+  </si>
+  <si>
+    <t>nexial.browserstack.browser</t>
+  </si>
+  <si>
+    <t>Chrome</t>
+  </si>
+  <si>
+    <t>nexial.browserstack.browser.version</t>
+  </si>
+  <si>
+    <t>77</t>
+  </si>
+  <si>
+    <t xml:space="preserve">nexial.browserstack.os </t>
+  </si>
+  <si>
+    <t>WINDOWS</t>
+  </si>
+  <si>
+    <t>nexial.browserstack.os.version</t>
+  </si>
+  <si>
+    <t>10</t>
+  </si>
+  <si>
+    <t>nexial.browserstack.enablelocal</t>
+  </si>
+  <si>
+    <t>nexial.browserstack.*</t>
   </si>
 </sst>
 </file>
@@ -711,10 +762,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AAA199"/>
+  <dimension ref="A1:AAA200"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="A21" sqref="A21:XFD21"/>
+    <sheetView tabSelected="1" topLeftCell="A15" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="125" workbookViewId="0">
+      <selection activeCell="C23" sqref="C23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.69921875" defaultRowHeight="16.5" x14ac:dyDescent="0.25"/>
@@ -740,7 +791,7 @@
         <v>6</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>3</v>
+        <v>49</v>
       </c>
       <c r="HA2" s="3"/>
       <c r="AAA2" s="3"/>
@@ -787,17 +838,17 @@
     </row>
     <row r="7" spans="1:703" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>11</v>
+        <v>50</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>0</v>
+        <v>51</v>
       </c>
       <c r="HA7" s="6"/>
       <c r="AAA7" s="7"/>
     </row>
     <row r="8" spans="1:703" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B8" s="4" t="s">
         <v>0</v>
@@ -807,130 +858,174 @@
     </row>
     <row r="9" spans="1:703" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>14</v>
+        <v>0</v>
       </c>
       <c r="HA9" s="6"/>
       <c r="AAA9" s="7"/>
     </row>
     <row r="10" spans="1:703" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>23</v>
+        <v>13</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>0</v>
+        <v>14</v>
       </c>
       <c r="HA10" s="6"/>
       <c r="AAA10" s="7"/>
     </row>
     <row r="11" spans="1:703" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>15</v>
+        <v>23</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>16</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="HA11" s="6"/>
+      <c r="AAA11" s="7"/>
     </row>
     <row r="12" spans="1:703" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
     </row>
     <row r="13" spans="1:703" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>0</v>
+        <v>18</v>
       </c>
     </row>
     <row r="14" spans="1:703" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>18</v>
+        <v>0</v>
       </c>
     </row>
     <row r="15" spans="1:703" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B15" s="4" t="s">
-        <v>30</v>
+        <v>18</v>
       </c>
     </row>
     <row r="16" spans="1:703" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="B16" s="4" t="s">
-        <v>22</v>
+        <v>30</v>
       </c>
     </row>
     <row r="17" spans="1:2" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="B17" s="4" t="s">
-        <v>0</v>
+        <v>22</v>
       </c>
     </row>
     <row r="18" spans="1:2" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
-        <v>25</v>
+        <v>29</v>
       </c>
       <c r="B18" s="4" t="s">
-        <v>26</v>
+        <v>0</v>
       </c>
     </row>
     <row r="19" spans="1:2" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B19" s="4" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
     </row>
     <row r="20" spans="1:2" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B20" s="4" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="B20" s="4" t="s">
+      <c r="B21" s="4" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:2" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="1"/>
-    </row>
     <row r="22" spans="1:2" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="1"/>
+      <c r="A22" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="B22" s="4" t="s">
+        <v>53</v>
+      </c>
     </row>
     <row r="23" spans="1:2" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="1"/>
+      <c r="A23" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="B23" s="4" t="s">
+        <v>55</v>
+      </c>
     </row>
     <row r="24" spans="1:2" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="1"/>
+      <c r="A24" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="B24" s="4" t="s">
+        <v>57</v>
+      </c>
     </row>
     <row r="25" spans="1:2" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="1"/>
+      <c r="A25" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="B25" s="4" t="s">
+        <v>59</v>
+      </c>
     </row>
     <row r="26" spans="1:2" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="1"/>
+      <c r="A26" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="B26" s="4" t="s">
+        <v>61</v>
+      </c>
     </row>
     <row r="27" spans="1:2" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="1"/>
+      <c r="A27" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="B27" s="4" t="s">
+        <v>63</v>
+      </c>
     </row>
     <row r="28" spans="1:2" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="1"/>
+      <c r="A28" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="B28" s="4" t="s">
+        <v>4</v>
+      </c>
     </row>
     <row r="29" spans="1:2" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="1"/>
+      <c r="A29" s="1" t="s">
+        <v>65</v>
+      </c>
     </row>
     <row r="30" spans="1:2" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="1"/>
@@ -1441,6 +1536,9 @@
     </row>
     <row r="199" spans="1:1" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A199" s="1"/>
+    </row>
+    <row r="200" spans="1:1" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A200" s="1"/>
     </row>
   </sheetData>
   <sheetProtection sheet="1" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" deleteColumns="0" deleteRows="0" sort="0"/>

</xml_diff>